<commit_message>
update build excel && added textures
</commit_message>
<xml_diff>
--- a/Excel/Build.xlsx
+++ b/Excel/Build.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -41,6 +41,12 @@
     <t>等级需求</t>
   </si>
   <si>
+    <t>按钮图片</t>
+  </si>
+  <si>
+    <t>贴图</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -53,6 +59,12 @@
     <t>level_need</t>
   </si>
   <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>texture</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
@@ -68,7 +80,10 @@
     <t>面包坊</t>
   </si>
   <si>
-    <t>2</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Buid_01</t>
   </si>
   <si>
     <t>400102</t>
@@ -1039,23 +1054,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="19.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.625" style="1" customWidth="1"/>
-    <col min="5" max="16375" width="9" style="1"/>
+    <col min="5" max="5" width="15.5833333333333" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" style="1" customWidth="1"/>
+    <col min="7" max="16375" width="9" style="1"/>
     <col min="16378" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26" customHeight="1" spans="1:4">
+    <row r="1" ht="26" customHeight="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,75 +1085,105 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="3:3">

</xml_diff>

<commit_message>
alter few fields name
</commit_message>
<xml_diff>
--- a/Excel/Build.xlsx
+++ b/Excel/Build.xlsx
@@ -4,13 +4,26 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="20460" windowHeight="13455"/>
+    <workbookView windowWidth="28800" windowHeight="14055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -65,10 +78,10 @@
     <t>png</t>
   </si>
   <si>
-    <t>coin</t>
+    <t>cost_coin</t>
   </si>
   <si>
-    <t>diamond</t>
+    <t>cost_diamond</t>
   </si>
   <si>
     <t>prosperity</t>
@@ -374,12 +387,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -403,81 +416,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -494,8 +432,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -510,8 +455,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -525,13 +494,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -540,8 +502,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -568,13 +581,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,7 +593,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,79 +629,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,13 +653,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -706,49 +743,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -866,6 +879,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -890,22 +927,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -925,21 +957,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -949,169 +966,165 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1138,9 +1151,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1153,52 +1163,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1472,10 +1482,10 @@
   <dimension ref="A1:O16384"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9" style="16"/>
     <col min="2" max="2" width="19.125" style="16" customWidth="1"/>
@@ -1483,7 +1493,11 @@
     <col min="4" max="4" width="18.625" style="16" customWidth="1"/>
     <col min="5" max="5" width="15.5833333333333" style="16" customWidth="1"/>
     <col min="6" max="6" width="17.25" style="16" customWidth="1"/>
-    <col min="7" max="16375" width="9" style="16"/>
+    <col min="7" max="7" width="9" style="16"/>
+    <col min="8" max="8" width="16.875" style="16" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="16" customWidth="1"/>
+    <col min="10" max="10" width="18.625" style="16" customWidth="1"/>
+    <col min="11" max="16375" width="9" style="16"/>
     <col min="16378" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
@@ -1509,18 +1523,18 @@
       <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="16"/>
       <c r="M1" s="16"/>
-      <c r="N1" s="18"/>
+      <c r="N1" s="17"/>
       <c r="O1" s="16"/>
     </row>
     <row r="2" customFormat="1" spans="1:15">
@@ -1551,22 +1565,22 @@
       <c r="I2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="16"/>
       <c r="M2" s="16"/>
-      <c r="N2" s="18"/>
+      <c r="N2" s="17"/>
       <c r="O2" s="16"/>
     </row>
     <row r="3" customFormat="1" spans="1:15">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="16" t="s">
@@ -1587,7 +1601,7 @@
       <c r="I3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="17" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="16"/>
@@ -1602,7 +1616,7 @@
       <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="16" t="s">
@@ -1638,7 +1652,7 @@
       <c r="B5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="16" t="s">
@@ -1651,10 +1665,10 @@
         <v>31</v>
       </c>
       <c r="G5" s="17"/>
-      <c r="H5" s="18">
+      <c r="H5" s="17">
         <v>20</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="17">
         <v>20</v>
       </c>
     </row>
@@ -1662,10 +1676,10 @@
       <c r="A6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -1674,14 +1688,14 @@
       <c r="E6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>35</v>
       </c>
       <c r="G6" s="17"/>
-      <c r="H6" s="18">
+      <c r="H6" s="17">
         <v>40</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="17">
         <v>40</v>
       </c>
     </row>
@@ -1705,11 +1719,11 @@
         <v>39</v>
       </c>
       <c r="G7"/>
-      <c r="H7" s="18">
+      <c r="H7" s="17">
         <v>80</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18">
+      <c r="I7" s="17"/>
+      <c r="J7" s="17">
         <v>80</v>
       </c>
     </row>
@@ -1720,7 +1734,7 @@
       <c r="B8" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>44</v>
       </c>
       <c r="D8" s="16" t="s">
@@ -1748,7 +1762,7 @@
       <c r="B9" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>49</v>
       </c>
       <c r="D9" s="16" t="s">
@@ -18585,7 +18599,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" ht="16.5" spans="1:17">
       <c r="A1" s="1"/>

</xml_diff>